<commit_message>
added transaction-reaction dataset, adjusted deal_id in transaction
</commit_message>
<xml_diff>
--- a/transactions.xlsx
+++ b/transactions.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xiaon\OneDrive\Thesis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cc5c22409b1431eb/Thesis/tongdu/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="576" documentId="8_{2E3C25A1-3809-4F01-8F7B-7692EFB976BB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{3322896E-92F6-4993-80A0-517F7BEBC8C5}"/>
+  <xr:revisionPtr revIDLastSave="626" documentId="8_{2E3C25A1-3809-4F01-8F7B-7692EFB976BB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{EB4979B1-1E8E-4F9C-AF37-244BF06B14A9}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{B7420A61-7754-4A14-B263-A040E7DE97EE}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="codebook" sheetId="7" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_4" localSheetId="0" hidden="1">transactions!$B$1:$D$111</definedName>
+    <definedName name="ExternalData_4" localSheetId="0" hidden="1">transactions!$B$1:$D$112</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="117">
   <si>
     <t>60 UH-60M Black Hawk helicopters with 120 T-700-GE-701D engines, etc.</t>
   </si>
@@ -403,6 +403,9 @@
   </si>
   <si>
     <t>assigned ID to each transaction; contracts announced or finalized within a week apart are considered one single deal to account for the fact that the CCP can only recact so many times in a week on the sam issue. This file only includes what the DSCA would consider as major weapon systems. Source: DSCA "Major Arms Sales" and Kan (2014) for CRS</t>
+  </si>
+  <si>
+    <t>bush approves the 4 Kidd-class destroyers</t>
   </si>
 </sst>
 </file>
@@ -410,7 +413,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyymmdd"/>
+    <numFmt numFmtId="164" formatCode="yyyymmdd"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -459,20 +462,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
     <dxf>
-      <numFmt numFmtId="165" formatCode="yyyymmdd"/>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="yyyymmdd"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -504,12 +507,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{B1A3A79E-07B1-4155-8E4C-6E3F8AA1A93F}" name="George_H__W__Bush__01_20_1989_01_20_1993__edit" displayName="George_H__W__Bush__01_20_1989_01_20_1993__edit" ref="A1:D111" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:D111" xr:uid="{FF046322-E505-4609-B55F-4BBAD28B2450}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{B1A3A79E-07B1-4155-8E4C-6E3F8AA1A93F}" name="George_H__W__Bush__01_20_1989_01_20_1993__edit" displayName="George_H__W__Bush__01_20_1989_01_20_1993__edit" ref="A1:D112" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:D112" xr:uid="{FF046322-E505-4609-B55F-4BBAD28B2450}"/>
   <tableColumns count="4">
-    <tableColumn id="6" xr3:uid="{22CB8E55-1954-4CA8-B8DA-C9B5C03E7160}" uniqueName="6" name="deal_id" queryTableFieldId="6" dataDxfId="1"/>
-    <tableColumn id="1" xr3:uid="{7A0A624A-A545-4C9F-B690-5775B460763F}" uniqueName="1" name="date" queryTableFieldId="1" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{1174096E-7C41-4F94-857B-DC174ECE6215}" uniqueName="2" name="items" queryTableFieldId="2" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{22CB8E55-1954-4CA8-B8DA-C9B5C03E7160}" uniqueName="6" name="deal_id" queryTableFieldId="6" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{7A0A624A-A545-4C9F-B690-5775B460763F}" uniqueName="1" name="date" queryTableFieldId="1" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{1174096E-7C41-4F94-857B-DC174ECE6215}" uniqueName="2" name="items" queryTableFieldId="2" dataDxfId="0"/>
     <tableColumn id="3" xr3:uid="{1889D366-D721-4176-A342-9C5BB915B360}" uniqueName="3" name="value_million" queryTableFieldId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -813,10 +816,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{130B9847-9D0E-4E78-968D-74AA7E6DE09B}">
-  <dimension ref="A1:D111"/>
+  <dimension ref="A1:D112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="C106" sqref="C106"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="C71" sqref="C71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -1768,16 +1771,13 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A68" s="3">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B68" s="7">
-        <v>37581</v>
+        <v>37005</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="D68">
-        <v>875</v>
+        <v>116</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.75">
@@ -1785,13 +1785,13 @@
         <v>46</v>
       </c>
       <c r="B69" s="7">
-        <v>37888</v>
+        <v>37581</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="D69">
-        <v>775</v>
+        <v>875</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.75">
@@ -1799,13 +1799,13 @@
         <v>47</v>
       </c>
       <c r="B70" s="7">
-        <v>38076</v>
+        <v>37888</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>57</v>
+        <v>95</v>
       </c>
       <c r="D70">
-        <v>1776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.75">
@@ -1813,13 +1813,13 @@
         <v>48</v>
       </c>
       <c r="B71" s="7">
-        <v>38650</v>
+        <v>38076</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>107</v>
+        <v>57</v>
       </c>
       <c r="D71">
-        <v>280</v>
+        <v>1776</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.75">
@@ -1827,13 +1827,13 @@
         <v>49</v>
       </c>
       <c r="B72" s="7">
-        <v>39141</v>
+        <v>38650</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D72">
-        <v>421</v>
+        <v>280</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.75">
@@ -1841,13 +1841,13 @@
         <v>50</v>
       </c>
       <c r="B73" s="7">
-        <v>39302</v>
+        <v>39141</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D73">
-        <v>125</v>
+        <v>421</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.75">
@@ -1855,27 +1855,27 @@
         <v>51</v>
       </c>
       <c r="B74" s="7">
-        <v>39337</v>
+        <v>39302</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D74">
-        <v>272</v>
+        <v>125</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A75" s="3">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B75" s="7">
         <v>39337</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>58</v>
+        <v>110</v>
       </c>
       <c r="D75">
-        <v>1960</v>
+        <v>272</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.75">
@@ -1883,13 +1883,13 @@
         <v>52</v>
       </c>
       <c r="B76" s="7">
-        <v>39395</v>
+        <v>39337</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D76">
-        <v>939</v>
+        <v>1960</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.75">
@@ -1897,83 +1897,83 @@
         <v>53</v>
       </c>
       <c r="B77" s="7">
-        <v>39724</v>
+        <v>39395</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D77">
-        <v>3100</v>
+        <v>939</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A78" s="3">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B78" s="7">
         <v>39724</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D78">
-        <v>200</v>
+        <v>3100</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A79" s="3">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B79" s="7">
         <v>39724</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="D79">
-        <v>334</v>
+        <v>200</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A80" s="3">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B80" s="7">
         <v>39724</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>112</v>
+        <v>49</v>
       </c>
       <c r="D80">
-        <v>47</v>
+        <v>334</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A81" s="3">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B81" s="7">
         <v>39724</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>62</v>
+        <v>112</v>
       </c>
       <c r="D81">
-        <v>250</v>
+        <v>47</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A82" s="3">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B82" s="7">
         <v>39724</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D82">
-        <v>2532</v>
+        <v>250</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.75">
@@ -1981,404 +1981,418 @@
         <v>54</v>
       </c>
       <c r="B83" s="7">
-        <v>40207</v>
+        <v>39724</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>0</v>
+        <v>63</v>
       </c>
       <c r="D83">
-        <v>3100</v>
+        <v>2532</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A84" s="3">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B84" s="7">
         <v>40207</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>113</v>
+        <v>0</v>
       </c>
       <c r="D84">
-        <v>340</v>
+        <v>3100</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A85" s="3">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B85" s="7">
         <v>40207</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>1</v>
+        <v>113</v>
       </c>
       <c r="D85">
-        <v>105</v>
+        <v>340</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A86" s="3">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B86" s="7">
         <v>40207</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>114</v>
+        <v>1</v>
       </c>
       <c r="D86">
-        <v>37</v>
+        <v>105</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A87" s="3">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B87" s="7">
         <v>40207</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>2</v>
+        <v>114</v>
       </c>
       <c r="D87">
-        <v>2810</v>
+        <v>37</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A88" s="3">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B88" s="7">
-        <v>40807</v>
+        <v>40207</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D88">
-        <v>500</v>
+        <v>2810</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A89" s="3">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B89" s="7">
         <v>40807</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D89">
-        <v>5300</v>
+        <v>500</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A90" s="3">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B90" s="7">
         <v>40807</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D90">
-        <v>52</v>
+        <v>5300</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A91" s="3">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B91" s="7">
-        <v>42354</v>
+        <v>40807</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D91">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A92" s="3">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B92" s="7">
         <v>42354</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D92">
-        <v>75</v>
+        <v>57</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A93" s="3">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B93" s="7">
         <v>42354</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D93">
-        <v>268</v>
+        <v>75</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A94" s="3">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B94" s="7">
         <v>42354</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D94">
-        <v>416</v>
+        <v>268</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A95" s="3">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B95" s="7">
         <v>42354</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D95">
-        <v>190</v>
+        <v>416</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A96" s="3">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B96" s="7">
         <v>42354</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D96">
-        <v>217</v>
+        <v>190</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A97" s="3">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B97" s="7">
         <v>42354</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D97">
-        <v>375</v>
+        <v>217</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A98" s="3">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B98" s="7">
         <v>42354</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D98">
-        <v>120</v>
+        <v>375</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A99" s="3">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B99" s="7">
         <v>42354</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D99">
-        <v>108</v>
+        <v>120</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A100" s="3">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B100" s="7">
-        <v>42915</v>
+        <v>42354</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="D100">
-        <v>125</v>
+        <v>108</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A101" s="3">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B101" s="7">
         <v>42915</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D101">
-        <v>175</v>
+        <v>125</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A102" s="3">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B102" s="7">
         <v>42915</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D102">
-        <v>250</v>
+        <v>175</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A103" s="3">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B103" s="7">
         <v>42915</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D103">
-        <v>80</v>
+        <v>250</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A104" s="3">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B104" s="7">
         <v>42915</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D104">
-        <v>185.5</v>
+        <v>80</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A105" s="3">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B105" s="7">
         <v>42915</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D105">
-        <v>147.5</v>
+        <v>185.5</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A106" s="3">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B106" s="7">
         <v>42915</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D106">
-        <v>400</v>
+        <v>147.5</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A107" s="3">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B107" s="7">
-        <v>43367</v>
+        <v>42915</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D107">
-        <v>330</v>
+        <v>400</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A108" s="3">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B108" s="7">
-        <v>43570</v>
+        <v>43367</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D108">
-        <v>500</v>
+        <v>330</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A109" s="3">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B109" s="7">
-        <v>43654</v>
+        <v>43570</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D109">
-        <v>223.56</v>
+        <v>500</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A110" s="3">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B110" s="7">
         <v>43654</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D110">
-        <v>2000</v>
+        <v>223.56</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A111" s="3">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B111" s="7">
+        <v>43654</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D111">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A112" s="3">
+        <v>62</v>
+      </c>
+      <c r="B112" s="7">
         <v>43697</v>
       </c>
-      <c r="C111" s="2" t="s">
+      <c r="C112" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D111">
+      <c r="D112">
         <v>8000</v>
       </c>
     </row>

</xml_diff>